<commit_message>
add-generic-systems create generic systems
</commit_message>
<xml_diff>
--- a/tests/fixtures/ApstraProvisiongTemplate.xlsx
+++ b/tests/fixtures/ApstraProvisiongTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ckim/Documents/Projects/ck-apstra-api/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E479908D-B44B-0C49-99E3-B0E8E62793FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BED7DB8-28F3-9844-9B89-DA3A512637CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-10000" yWindow="-24880" windowWidth="37920" windowHeight="12280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="49">
   <si>
     <t>switch1</t>
   </si>
@@ -158,6 +158,15 @@
   </si>
   <si>
     <t>vn100-untagged, vn100-102</t>
+  </si>
+  <si>
+    <t>connectivity_template</t>
+  </si>
+  <si>
+    <t>untagged_vlan</t>
+  </si>
+  <si>
+    <t>tagged_vlans</t>
   </si>
 </sst>
 </file>
@@ -212,7 +221,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -222,149 +231,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color auto="1"/>
       </right>
-      <top style="thick">
-        <color rgb="FF000000"/>
+      <top style="thin">
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFC6C6C6"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFC6C6C6"/>
-      </right>
-      <top style="thick">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFC6C6C6"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thick">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thick">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thick">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thick">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thick">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFC6C6C6"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -372,78 +248,44 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -749,10 +591,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:T8"/>
+  <dimension ref="A1:V8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S7" sqref="S7"/>
+      <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -767,270 +609,323 @@
     <col min="14" max="15" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="16.5" bestFit="1" customWidth="1"/>
     <col min="17" max="18" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="24" style="19" customWidth="1"/>
-    <col min="20" max="20" width="13" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="10.83203125" customWidth="1"/>
+    <col min="21" max="21" width="24" style="1" customWidth="1"/>
+    <col min="22" max="22" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="18.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="20"/>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="23" t="s">
+    <row r="1" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23" t="s">
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23" t="s">
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23" t="s">
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="3"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="3"/>
     </row>
-    <row r="2" spans="1:20" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="Q2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="R2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="S2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="U2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="T2" s="6" t="s">
+      <c r="V2" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="K3" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="L3" s="8" t="s">
+      <c r="L3" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="M3" s="10" t="s">
+      <c r="M3" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="N3" s="10" t="s">
+      <c r="N3" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="O3" s="8" t="s">
+      <c r="O3" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="P3" s="11" t="s">
+      <c r="P3" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="Q3" s="11" t="s">
+      <c r="Q3" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="R3" s="8" t="s">
+      <c r="R3" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="S3" s="12" t="s">
+      <c r="S3" s="6"/>
+      <c r="T3" s="6"/>
+      <c r="U3" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="T3" s="12"/>
+      <c r="V3" s="10"/>
     </row>
-    <row r="4" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="13" t="s">
+    <row r="4" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="14" t="s">
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="I4" s="14"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="16"/>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="17"/>
-      <c r="R4" s="17"/>
-      <c r="S4" s="24" t="s">
+      <c r="I4" s="6"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="T4" s="18"/>
+      <c r="V4" s="12"/>
     </row>
-    <row r="5" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="13" t="s">
+    <row r="5" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="14" t="s">
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="I5" s="14"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="16"/>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="17"/>
-      <c r="R5" s="17"/>
-      <c r="S5" s="19" t="s">
+      <c r="I5" s="6"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="9"/>
+      <c r="U5" s="13" t="s">
         <v>45</v>
       </c>
+      <c r="V5" s="14"/>
     </row>
-    <row r="6" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="D6" t="s">
+      <c r="C6" s="14"/>
+      <c r="D6" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="G6" t="s">
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="14" t="s">
         <v>43</v>
       </c>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
+      <c r="S6" s="14"/>
+      <c r="T6" s="14"/>
+      <c r="U6" s="13"/>
+      <c r="V6" s="14"/>
     </row>
-    <row r="7" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="D7" t="s">
+      <c r="C7" s="14"/>
+      <c r="D7" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="G7" t="s">
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="14" t="s">
         <v>43</v>
       </c>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="14"/>
+      <c r="S7" s="14"/>
+      <c r="T7" s="14"/>
+      <c r="U7" s="13"/>
+      <c r="V7" s="14"/>
     </row>
-    <row r="8" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="S1:U1"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="J1:L1"/>

</xml_diff>

<commit_message>
implement rz loopback_ip pool
</commit_message>
<xml_diff>
--- a/tests/fixtures/ApstraProvisiongTemplate.xlsx
+++ b/tests/fixtures/ApstraProvisiongTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ckim/Documents/Projects/ck-apstra-api/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{528DD396-01CE-EB41-BF07-4B10DDF09B60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30EB6595-5616-DF4B-9C9A-9581742AE4A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11040" yWindow="-16520" windowWidth="37920" windowHeight="12280" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11040" yWindow="-16520" windowWidth="37920" windowHeight="12280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="routing_zones" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="105">
   <si>
     <t>switch1</t>
   </si>
@@ -306,6 +306,9 @@
     <t>Default_immutable</t>
   </si>
   <si>
+    <t>loopback_ips</t>
+  </si>
+  <si>
     <t>untagged</t>
   </si>
   <si>
@@ -331,6 +334,9 @@
   </si>
   <si>
     <t>multi-tagged</t>
+  </si>
+  <si>
+    <t>terra-loop</t>
   </si>
 </sst>
 </file>
@@ -477,7 +483,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -529,9 +535,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -837,10 +840,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A3C0123-44B8-744A-B78A-C0D06F1D7367}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -854,7 +857,7 @@
     <col min="7" max="16384" width="10.83203125" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
         <v>87</v>
       </c>
@@ -873,8 +876,11 @@
       <c r="F1" s="18" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="18" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
         <v>70</v>
       </c>
@@ -887,8 +893,11 @@
       <c r="D2" s="18" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" s="18" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
         <v>80</v>
       </c>
@@ -900,6 +909,9 @@
       </c>
       <c r="D3" s="18" t="s">
         <v>93</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1167,8 +1179,8 @@
   </sheetPr>
   <dimension ref="A1:Z9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1469,7 +1481,7 @@
         <v>23</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C6" s="13"/>
       <c r="D6" s="13" t="s">
@@ -1507,7 +1519,7 @@
         <v>23</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="13" t="s">
@@ -1545,52 +1557,84 @@
         <v>23</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D8" s="19" t="s">
         <v>26</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="G8" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="H8" s="21" t="s">
+      <c r="G8" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="H8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="I8" t="s">
-        <v>96</v>
-      </c>
-      <c r="W8">
+      <c r="I8" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="13"/>
+      <c r="S8" s="13"/>
+      <c r="T8" s="13"/>
+      <c r="U8" s="13"/>
+      <c r="V8" s="13"/>
+      <c r="W8" s="13">
         <v>100</v>
       </c>
+      <c r="X8" s="13"/>
+      <c r="Y8" s="12"/>
+      <c r="Z8" s="13"/>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
         <v>23</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D9" s="19" t="s">
         <v>26</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="G9" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="H9" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="H9" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="I9" t="s">
-        <v>96</v>
-      </c>
-      <c r="X9" t="s">
-        <v>100</v>
-      </c>
+      <c r="I9" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13"/>
+      <c r="S9" s="13"/>
+      <c r="T9" s="13"/>
+      <c r="U9" s="13"/>
+      <c r="V9" s="13"/>
+      <c r="W9" s="13"/>
+      <c r="X9" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y9" s="12"/>
+      <c r="Z9" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>